<commit_message>
modified figures, added descriptive stats, table of plants, sample sizes for ridgeplots.
</commit_message>
<xml_diff>
--- a/data/adonis_results.xlsx
+++ b/data/adonis_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riley\Desktop\CrowderLab\Camille\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCE530D5-B062-41A0-84DC-187D29598031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F76E72DB-5A4E-4D55-9BFE-54728F5C6320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{29252103-6EA4-47FE-819A-DB9D131C47A1}"/>
   </bookViews>
@@ -987,7 +987,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection sqref="A1:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>